<commit_message>
Fix plan de masse grand robot
</commit_message>
<xml_diff>
--- a/Pôle mécatronique/Electronique/Documents informatif/BOM/BOM.xlsx
+++ b/Pôle mécatronique/Electronique/Documents informatif/BOM/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomro\OneDrive\Documents\GitHub\2021-2022\Pôle mécatronique\Electronique\Documents informatif\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\2021-2022\Pôle mécatronique\Electronique\Documents informatif\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7F076B-2A92-41DD-B33E-36E713A7BD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98ECDE36-4ADA-4BEB-818A-AD74E2B7921F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{855F23A4-F16C-4481-B3A5-88449A0A64F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{855F23A4-F16C-4481-B3A5-88449A0A64F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Version Kicad" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="259">
   <si>
     <t>Id</t>
   </si>
@@ -584,9 +584,6 @@
     <t>Interrupteur</t>
   </si>
   <si>
-    <t>XT30</t>
-  </si>
-  <si>
     <t>Dupont x4</t>
   </si>
   <si>
@@ -633,12 +630,6 @@
   </si>
   <si>
     <t>Dupont 2x2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connecteurs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JST : </t>
   </si>
   <si>
     <t>x2</t>
@@ -789,12 +780,57 @@
   <si>
     <t>22pF</t>
   </si>
+  <si>
+    <t>C. connecteur</t>
+  </si>
+  <si>
+    <t>Colonne1</t>
+  </si>
+  <si>
+    <t>Colonne2</t>
+  </si>
+  <si>
+    <t>Colonne3</t>
+  </si>
+  <si>
+    <t>Colonne4</t>
+  </si>
+  <si>
+    <t>Colonne5</t>
+  </si>
+  <si>
+    <t>Colonne6</t>
+  </si>
+  <si>
+    <t>Colonne7</t>
+  </si>
+  <si>
+    <t>Colonne8</t>
+  </si>
+  <si>
+    <t>Colonne9</t>
+  </si>
+  <si>
+    <t>Colonne10</t>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>Connecteurs :</t>
+  </si>
+  <si>
+    <t>Par robot :</t>
+  </si>
+  <si>
+    <t>Colonne11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -807,6 +843,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -964,7 +1006,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -975,6 +1024,107 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E4036CF7-D54E-4D02-B817-847FD5874099}" name="Tableau5" displayName="Tableau5" ref="G4:Q10" totalsRowShown="0">
+  <autoFilter ref="G4:Q10" xr:uid="{E4036CF7-D54E-4D02-B817-847FD5874099}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{CEF682AD-F780-43E0-8472-AD0823558502}" name="Colonne1"/>
+    <tableColumn id="2" xr3:uid="{E20F4D22-06F9-491D-9568-1533B38BA819}" name="Colonne2"/>
+    <tableColumn id="3" xr3:uid="{61F27E79-B36E-4FB4-A7E3-AC27C7A7F52F}" name="Colonne3"/>
+    <tableColumn id="4" xr3:uid="{3A761683-FACD-4913-8838-0F516EE7274D}" name="Colonne4"/>
+    <tableColumn id="5" xr3:uid="{2B0279D5-B024-46A4-B99A-CD48953F8D75}" name="Colonne5"/>
+    <tableColumn id="6" xr3:uid="{ABCCDCDE-69B9-4482-93D9-5C4AFC50F8E1}" name="Colonne6"/>
+    <tableColumn id="7" xr3:uid="{47E3A175-1C0B-4951-9463-66B2B2BE57F1}" name="Colonne7"/>
+    <tableColumn id="8" xr3:uid="{25138F4B-967F-4606-A45E-C2DC763C9299}" name="Colonne8"/>
+    <tableColumn id="9" xr3:uid="{0A6C6788-38EC-48F0-8992-9D9070458B94}" name="Colonne9"/>
+    <tableColumn id="10" xr3:uid="{F90BC70A-9697-4C8E-BC71-1C5EE31BBC65}" name="Colonne10">
+      <calculatedColumnFormula>SUM(H5:O5)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{EAA80AC3-871A-4E43-8141-6A5779E49D6B}" name="Colonne11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0CFF9EA1-4B1B-4BE3-9788-AD644E07DC11}" name="Tableau6" displayName="Tableau6" ref="G17:P18" totalsRowShown="0">
+  <autoFilter ref="G17:P18" xr:uid="{0CFF9EA1-4B1B-4BE3-9788-AD644E07DC11}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{21496C46-B154-4D92-A583-D1CE13C5CBF9}" name="Colonne1"/>
+    <tableColumn id="2" xr3:uid="{22912ED9-DC48-4009-AD42-75E0B9B2B3C2}" name="BR">
+      <calculatedColumnFormula>30+32+16</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{94A239B5-8F84-4557-934D-205FEA590054}" name="Alim">
+      <calculatedColumnFormula>20</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{B5D23A4A-30D0-4030-9FB1-5D9E65E11980}" name="Hat">
+      <calculatedColumnFormula>40+4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{CA7EBE13-E0D5-4A53-BAFF-9AF347438141}" name="Petit">
+      <calculatedColumnFormula>2+30+16</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{7132B926-43A2-446B-9C39-F768EC65DC3D}" name="Grand"/>
+    <tableColumn id="7" xr3:uid="{8863BA3A-EB03-497C-B74F-4FBDABDF3685}" name="Odo">
+      <calculatedColumnFormula>30+15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{7E80951B-A75E-44F4-A71E-17B4DF947706}" name="Autres"/>
+    <tableColumn id="9" xr3:uid="{2E52F5E1-D1A4-467D-908D-CFB85D41CD96}" name="Par robot :">
+      <calculatedColumnFormula>SUM(H18:M18)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{641A9513-27A5-42AD-864D-2077BC12D45C}" name="Total :">
+      <calculatedColumnFormula>2*Tableau6[[#This Row],[Par robot :]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{34857799-3DE3-4E99-88BC-88F3F0387294}" name="Tableau8" displayName="Tableau8" ref="G24:P29" totalsRowShown="0">
+  <autoFilter ref="G24:P29" xr:uid="{34857799-3DE3-4E99-88BC-88F3F0387294}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{A976BA44-AECA-4450-9357-CBFA7ADD4A71}" name="Résistance : "/>
+    <tableColumn id="2" xr3:uid="{55D1CF1B-E4BB-4C53-8FE7-5D32967DBF58}" name="BR"/>
+    <tableColumn id="3" xr3:uid="{A0163128-0183-4B30-A3E1-41741DF59DA6}" name="Alim"/>
+    <tableColumn id="4" xr3:uid="{036FB7BA-1357-4214-B976-9FD1BE642D6B}" name="Hat"/>
+    <tableColumn id="5" xr3:uid="{BC85EFFC-9A92-470F-89CB-EC7FC52960F6}" name="Petit"/>
+    <tableColumn id="6" xr3:uid="{9CF8143B-5085-41FC-B14F-A1D493660CE2}" name="Grand"/>
+    <tableColumn id="7" xr3:uid="{649D5586-DB72-4C85-82BB-FC2EF5089663}" name="Odo"/>
+    <tableColumn id="8" xr3:uid="{AE264CB6-69D9-4A21-82BD-DD8404E70BEA}" name="Autres"/>
+    <tableColumn id="9" xr3:uid="{E3AA1989-83C6-4340-A5FE-29E19A18FBB1}" name="Par robot :">
+      <calculatedColumnFormula>SUM(H25:N25)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{A81EBA1C-ABF8-4362-9585-9222E620EBBF}" name="Total :" dataDxfId="1">
+      <calculatedColumnFormula>2*Tableau8[[#This Row],[Par robot :]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{650AACBF-9F8F-41BB-91C8-588D94D7F33B}" name="Tableau9" displayName="Tableau9" ref="G34:P40" totalsRowShown="0">
+  <autoFilter ref="G34:P40" xr:uid="{650AACBF-9F8F-41BB-91C8-588D94D7F33B}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{9F887D04-9583-40CD-AED4-6BF985441896}" name="Condensateur : "/>
+    <tableColumn id="2" xr3:uid="{8FF03F7B-E778-4595-B375-8E5AA47C0FEA}" name="BR"/>
+    <tableColumn id="3" xr3:uid="{0AF2613C-F2F4-4EFB-9BC6-077EE7203769}" name="Alim"/>
+    <tableColumn id="4" xr3:uid="{8223C7F7-FA12-4EFA-A379-0A9E02D97E7A}" name="Hat"/>
+    <tableColumn id="5" xr3:uid="{7FA5F7A7-E526-4598-92E1-8F1A2A135154}" name="Petit"/>
+    <tableColumn id="6" xr3:uid="{55556819-7A02-44B1-86CD-05B62D044D82}" name="Grand"/>
+    <tableColumn id="7" xr3:uid="{7F141C09-3B4F-41FB-8B5E-68CEFE800220}" name="Odo"/>
+    <tableColumn id="8" xr3:uid="{6F92780A-9BAA-4BFB-A496-5749F15F0FB7}" name="Autres"/>
+    <tableColumn id="9" xr3:uid="{1E15E7C1-C1B5-426C-8F86-6661686B8AB9}" name="Par robot :">
+      <calculatedColumnFormula>SUM(H35:N35)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{DD591600-FDED-42A4-87E9-E0182301B319}" name="Total :" dataDxfId="0">
+      <calculatedColumnFormula>2*Tableau9[[#This Row],[Par robot :]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1280,20 +1430,20 @@
       <selection activeCell="A113" sqref="A113:E126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="68.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1330,7 +1480,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1347,7 +1497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1364,7 +1514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1381,7 +1531,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1398,7 +1548,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1415,7 +1565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1432,7 +1582,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1449,7 +1599,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1466,7 +1616,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1483,7 +1633,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1500,7 +1650,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1517,7 +1667,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1534,7 +1684,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1551,7 +1701,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1568,7 +1718,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1585,7 +1735,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1602,7 +1752,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1619,12 +1769,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1641,7 +1791,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1658,7 +1808,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1675,7 +1825,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1692,7 +1842,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1709,7 +1859,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1726,7 +1876,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1743,7 +1893,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7</v>
       </c>
@@ -1760,7 +1910,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>8</v>
       </c>
@@ -1777,7 +1927,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9</v>
       </c>
@@ -1794,7 +1944,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>10</v>
       </c>
@@ -1811,7 +1961,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>11</v>
       </c>
@@ -1828,7 +1978,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>12</v>
       </c>
@@ -1845,7 +1995,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>13</v>
       </c>
@@ -1862,7 +2012,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>14</v>
       </c>
@@ -1879,7 +2029,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>15</v>
       </c>
@@ -1896,7 +2046,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>16</v>
       </c>
@@ -1913,7 +2063,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>17</v>
       </c>
@@ -1930,7 +2080,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>18</v>
       </c>
@@ -1947,7 +2097,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>19</v>
       </c>
@@ -1964,7 +2114,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>20</v>
       </c>
@@ -1981,12 +2131,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -2003,7 +2153,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -2017,7 +2167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -2034,7 +2184,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2051,7 +2201,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -2068,7 +2218,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2085,7 +2235,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6</v>
       </c>
@@ -2102,7 +2252,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7</v>
       </c>
@@ -2119,7 +2269,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>8</v>
       </c>
@@ -2136,7 +2286,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9</v>
       </c>
@@ -2153,7 +2303,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>10</v>
       </c>
@@ -2170,7 +2320,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>11</v>
       </c>
@@ -2187,7 +2337,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>12</v>
       </c>
@@ -2204,7 +2354,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>13</v>
       </c>
@@ -2221,7 +2371,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>14</v>
       </c>
@@ -2238,7 +2388,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>15</v>
       </c>
@@ -2255,7 +2405,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>16</v>
       </c>
@@ -2272,7 +2422,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>17</v>
       </c>
@@ -2289,7 +2439,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>18</v>
       </c>
@@ -2306,7 +2456,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>19</v>
       </c>
@@ -2323,12 +2473,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -2345,7 +2495,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1</v>
       </c>
@@ -2362,7 +2512,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2</v>
       </c>
@@ -2379,7 +2529,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>3</v>
       </c>
@@ -2396,7 +2546,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>4</v>
       </c>
@@ -2413,7 +2563,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>5</v>
       </c>
@@ -2430,7 +2580,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>6</v>
       </c>
@@ -2447,7 +2597,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>7</v>
       </c>
@@ -2464,7 +2614,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>8</v>
       </c>
@@ -2481,7 +2631,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>9</v>
       </c>
@@ -2498,7 +2648,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>10</v>
       </c>
@@ -2515,7 +2665,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>11</v>
       </c>
@@ -2532,7 +2682,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>12</v>
       </c>
@@ -2549,7 +2699,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>13</v>
       </c>
@@ -2566,7 +2716,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>14</v>
       </c>
@@ -2583,7 +2733,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>15</v>
       </c>
@@ -2600,7 +2750,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>16</v>
       </c>
@@ -2617,7 +2767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>17</v>
       </c>
@@ -2634,7 +2784,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>18</v>
       </c>
@@ -2651,7 +2801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>19</v>
       </c>
@@ -2668,7 +2818,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>20</v>
       </c>
@@ -2685,7 +2835,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>21</v>
       </c>
@@ -2702,7 +2852,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>22</v>
       </c>
@@ -2719,12 +2869,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -2741,7 +2891,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1</v>
       </c>
@@ -2752,7 +2902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2</v>
       </c>
@@ -2769,7 +2919,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>3</v>
       </c>
@@ -2786,7 +2936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>4</v>
       </c>
@@ -2803,7 +2953,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>5</v>
       </c>
@@ -2820,7 +2970,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>6</v>
       </c>
@@ -2837,7 +2987,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>7</v>
       </c>
@@ -2854,7 +3004,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>8</v>
       </c>
@@ -2871,7 +3021,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>9</v>
       </c>
@@ -2888,7 +3038,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>10</v>
       </c>
@@ -2905,7 +3055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>11</v>
       </c>
@@ -2922,7 +3072,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>12</v>
       </c>
@@ -2939,7 +3089,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>13</v>
       </c>
@@ -2956,7 +3106,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>14</v>
       </c>
@@ -2973,7 +3123,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>15</v>
       </c>
@@ -2990,7 +3140,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>16</v>
       </c>
@@ -3007,7 +3157,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>17</v>
       </c>
@@ -3024,12 +3174,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>0</v>
       </c>
@@ -3046,12 +3196,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1</v>
       </c>
       <c r="B115" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C115" t="s">
         <v>77</v>
@@ -3063,12 +3213,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2</v>
       </c>
       <c r="B116" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C116" t="s">
         <v>54</v>
@@ -3080,29 +3230,29 @@
         <v>55</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>3</v>
       </c>
       <c r="B117" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C117" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D117">
         <v>1</v>
       </c>
       <c r="E117" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>4</v>
       </c>
       <c r="B118" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C118" t="s">
         <v>57</v>
@@ -3114,7 +3264,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>5</v>
       </c>
@@ -3122,16 +3272,16 @@
         <v>17</v>
       </c>
       <c r="C119" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D119">
         <v>1</v>
       </c>
       <c r="E119" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>6</v>
       </c>
@@ -3148,12 +3298,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>7</v>
       </c>
       <c r="B121" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C121" t="s">
         <v>3</v>
@@ -3165,7 +3315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>8</v>
       </c>
@@ -3173,16 +3323,16 @@
         <v>127</v>
       </c>
       <c r="C122" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D122">
         <v>1</v>
       </c>
       <c r="E122" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>9</v>
       </c>
@@ -3199,12 +3349,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>10</v>
       </c>
       <c r="B124" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C124" t="s">
         <v>79</v>
@@ -3216,12 +3366,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>11</v>
       </c>
       <c r="B125" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C125" t="s">
         <v>33</v>
@@ -3233,12 +3383,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>12</v>
       </c>
       <c r="B126" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C126" t="s">
         <v>102</v>
@@ -3257,29 +3407,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7BCE7D-E3CC-4260-8BD3-B5A1313CB237}">
-  <dimension ref="A1:O110"/>
+  <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3296,10 +3451,10 @@
         <v>175</v>
       </c>
       <c r="G2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -3315,32 +3470,8 @@
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" t="s">
-        <v>225</v>
-      </c>
-      <c r="J3" t="s">
-        <v>226</v>
-      </c>
-      <c r="K3" t="s">
-        <v>227</v>
-      </c>
-      <c r="L3" t="s">
-        <v>228</v>
-      </c>
-      <c r="M3" t="s">
-        <v>203</v>
-      </c>
-      <c r="N3" t="s">
-        <v>231</v>
-      </c>
-      <c r="O3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -3354,13 +3485,43 @@
         <v>4</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+      <c r="H4" t="s">
+        <v>246</v>
+      </c>
+      <c r="I4" t="s">
+        <v>247</v>
+      </c>
+      <c r="J4" t="s">
+        <v>248</v>
+      </c>
+      <c r="K4" t="s">
+        <v>249</v>
+      </c>
+      <c r="L4" t="s">
+        <v>250</v>
+      </c>
+      <c r="M4" t="s">
+        <v>251</v>
+      </c>
+      <c r="N4" t="s">
+        <v>252</v>
+      </c>
+      <c r="O4" t="s">
+        <v>253</v>
+      </c>
+      <c r="P4" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -3377,30 +3538,40 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>201</v>
-      </c>
-      <c r="H5">
-        <f>D12</f>
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <f>SUM(H5:N5)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>222</v>
+      </c>
+      <c r="J5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K5" t="s">
+        <v>224</v>
+      </c>
+      <c r="L5" t="s">
+        <v>225</v>
+      </c>
+      <c r="M5" t="s">
+        <v>200</v>
+      </c>
+      <c r="N5" t="s">
+        <v>244</v>
+      </c>
+      <c r="O5" t="s">
+        <v>228</v>
+      </c>
+      <c r="P5" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -3417,20 +3588,34 @@
         <v>180</v>
       </c>
       <c r="G6" t="s">
-        <v>202</v>
+        <v>198</v>
+      </c>
+      <c r="H6">
+        <f>D12</f>
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
       </c>
       <c r="K6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>2</v>
-      </c>
-      <c r="O6">
-        <f t="shared" ref="O6:O9" si="0">SUM(H6:N6)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <f>SUM(H6:O6)</f>
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <f>2*Tableau5[[#This Row],[Colonne10]]</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -3447,64 +3632,74 @@
         <v>181</v>
       </c>
       <c r="G7" t="s">
-        <v>222</v>
-      </c>
-      <c r="I7">
+        <v>199</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <f>SUM(H7:O7)</f>
+        <v>11</v>
+      </c>
+      <c r="Q7">
+        <f>2*Tableau5[[#This Row],[Colonne10]]</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="G8" t="s">
+        <v>219</v>
+      </c>
+      <c r="I8">
         <f>D22</f>
         <v>3</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>2</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="G8" t="s">
-        <v>223</v>
-      </c>
-      <c r="I8">
-        <f>D23</f>
-        <v>2</v>
+      <c r="J8">
+        <v>1</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
       <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <f>SUM(H8:O8)</f>
+        <v>8</v>
+      </c>
+      <c r="Q8">
+        <f>2*Tableau5[[#This Row],[Colonne10]]</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>9</v>
       </c>
@@ -3521,17 +3716,34 @@
         <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>224</v>
+        <v>220</v>
+      </c>
+      <c r="I9">
+        <f>D23</f>
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
       </c>
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <f>SUM(H9:O9)</f>
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <f>2*Tableau5[[#This Row],[Colonne10]]</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>10</v>
       </c>
@@ -3547,8 +3759,22 @@
       <c r="E10" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>221</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f>SUM(H10:O10)</f>
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <f>2*Tableau5[[#This Row],[Colonne10]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>12</v>
       </c>
@@ -3564,11 +3790,8 @@
       <c r="E11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>13</v>
       </c>
@@ -3582,10 +3805,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>14</v>
       </c>
@@ -3602,7 +3825,7 @@
         <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -3611,7 +3834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>15</v>
       </c>
@@ -3628,7 +3851,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>16</v>
       </c>
@@ -3645,35 +3868,41 @@
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>245</v>
+      </c>
       <c r="H17" t="s">
         <v>51</v>
       </c>
       <c r="I17" t="s">
+        <v>222</v>
+      </c>
+      <c r="J17" t="s">
+        <v>223</v>
+      </c>
+      <c r="K17" t="s">
+        <v>224</v>
+      </c>
+      <c r="L17" t="s">
         <v>225</v>
       </c>
-      <c r="J17" t="s">
+      <c r="M17" t="s">
+        <v>200</v>
+      </c>
+      <c r="N17" t="s">
+        <v>228</v>
+      </c>
+      <c r="O17" t="s">
+        <v>257</v>
+      </c>
+      <c r="P17" t="s">
         <v>226</v>
       </c>
-      <c r="K17" t="s">
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
         <v>227</v>
-      </c>
-      <c r="L17" t="s">
-        <v>228</v>
-      </c>
-      <c r="M17" t="s">
-        <v>203</v>
-      </c>
-      <c r="N17" t="s">
-        <v>231</v>
-      </c>
-      <c r="O17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G18" t="s">
-        <v>230</v>
       </c>
       <c r="H18">
         <f>30+32+16</f>
@@ -3702,14 +3931,18 @@
         <f>SUM(H18:M18)</f>
         <v>265</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P18">
+        <f>2*Tableau6[[#This Row],[Par robot :]]</f>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>0</v>
       </c>
@@ -3726,7 +3959,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>1</v>
       </c>
@@ -3740,10 +3973,10 @@
         <v>3</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>2</v>
       </c>
@@ -3757,34 +3990,10 @@
         <v>2</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="H23" t="s">
-        <v>51</v>
-      </c>
-      <c r="I23" t="s">
-        <v>225</v>
-      </c>
-      <c r="J23" t="s">
-        <v>226</v>
-      </c>
-      <c r="K23" t="s">
-        <v>227</v>
-      </c>
-      <c r="L23" t="s">
-        <v>228</v>
-      </c>
-      <c r="M23" t="s">
-        <v>203</v>
-      </c>
-      <c r="N23" t="s">
-        <v>231</v>
-      </c>
-      <c r="O23" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>3</v>
       </c>
@@ -3801,10 +4010,37 @@
         <v>61</v>
       </c>
       <c r="G24" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+      <c r="H24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" t="s">
+        <v>222</v>
+      </c>
+      <c r="J24" t="s">
+        <v>223</v>
+      </c>
+      <c r="K24" t="s">
+        <v>224</v>
+      </c>
+      <c r="L24" t="s">
+        <v>225</v>
+      </c>
+      <c r="M24" t="s">
+        <v>200</v>
+      </c>
+      <c r="N24" t="s">
+        <v>228</v>
+      </c>
+      <c r="O24" t="s">
+        <v>257</v>
+      </c>
+      <c r="P24" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>4</v>
       </c>
@@ -3821,7 +4057,7 @@
         <v>64</v>
       </c>
       <c r="G25" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I25">
         <v>2</v>
@@ -3830,8 +4066,12 @@
         <f>SUM(H25:N25)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <f>2*Tableau8[[#This Row],[Par robot :]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>5</v>
       </c>
@@ -3848,17 +4088,21 @@
         <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K26">
         <v>1</v>
       </c>
       <c r="O26">
-        <f t="shared" ref="O26:O29" si="1">SUM(H26:N26)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+        <f>SUM(H26:N26)</f>
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <f>2*Tableau8[[#This Row],[Par robot :]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>6</v>
       </c>
@@ -3872,10 +4116,10 @@
         <v>1</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G27" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -3884,11 +4128,15 @@
         <v>1</v>
       </c>
       <c r="O27">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+        <f>SUM(H27:N27)</f>
+        <v>2</v>
+      </c>
+      <c r="P27">
+        <f>2*Tableau8[[#This Row],[Par robot :]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>7</v>
       </c>
@@ -3902,20 +4150,24 @@
         <v>1</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G28" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="J28">
         <v>1</v>
       </c>
       <c r="O28">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+        <f>SUM(H28:N28)</f>
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <f>2*Tableau8[[#This Row],[Par robot :]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>8</v>
       </c>
@@ -3929,10 +4181,10 @@
         <v>1</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G29" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K29">
         <v>2</v>
@@ -3941,11 +4193,15 @@
         <v>2</v>
       </c>
       <c r="O29">
-        <f t="shared" si="1"/>
+        <f>SUM(H29:N29)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29">
+        <f>2*Tableau8[[#This Row],[Par robot :]]</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>9</v>
       </c>
@@ -3962,7 +4218,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>11</v>
       </c>
@@ -3976,10 +4232,10 @@
         <v>1</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>12</v>
       </c>
@@ -3993,10 +4249,10 @@
         <v>1</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>14</v>
       </c>
@@ -4012,32 +4268,8 @@
       <c r="E33" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="H33" t="s">
-        <v>51</v>
-      </c>
-      <c r="I33" t="s">
-        <v>225</v>
-      </c>
-      <c r="J33" t="s">
-        <v>226</v>
-      </c>
-      <c r="K33" t="s">
-        <v>227</v>
-      </c>
-      <c r="L33" t="s">
-        <v>228</v>
-      </c>
-      <c r="M33" t="s">
-        <v>203</v>
-      </c>
-      <c r="N33" t="s">
-        <v>231</v>
-      </c>
-      <c r="O33" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>15</v>
       </c>
@@ -4051,13 +4283,40 @@
         <v>1</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G34" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+      <c r="H34" t="s">
+        <v>51</v>
+      </c>
+      <c r="I34" t="s">
+        <v>222</v>
+      </c>
+      <c r="J34" t="s">
+        <v>223</v>
+      </c>
+      <c r="K34" t="s">
+        <v>224</v>
+      </c>
+      <c r="L34" t="s">
+        <v>225</v>
+      </c>
+      <c r="M34" t="s">
+        <v>200</v>
+      </c>
+      <c r="N34" t="s">
+        <v>228</v>
+      </c>
+      <c r="O34" t="s">
+        <v>257</v>
+      </c>
+      <c r="P34" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>16</v>
       </c>
@@ -4074,7 +4333,7 @@
         <v>91</v>
       </c>
       <c r="G35" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H35">
         <v>4</v>
@@ -4086,8 +4345,12 @@
         <f>SUM(H35:N35)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P35">
+        <f>2*Tableau9[[#This Row],[Par robot :]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>17</v>
       </c>
@@ -4104,17 +4367,21 @@
         <v>93</v>
       </c>
       <c r="G36" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="J36">
         <v>2</v>
       </c>
       <c r="O36">
-        <f t="shared" ref="O36:O40" si="2">SUM(H36:N36)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" ref="O36:O40" si="0">SUM(H36:N36)</f>
+        <v>2</v>
+      </c>
+      <c r="P36">
+        <f>2*Tableau9[[#This Row],[Par robot :]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>18</v>
       </c>
@@ -4146,11 +4413,15 @@
         <v>2</v>
       </c>
       <c r="O37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37">
+        <f>2*Tableau9[[#This Row],[Par robot :]]</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>20</v>
       </c>
@@ -4164,7 +4435,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G38" t="s">
         <v>45</v>
@@ -4185,38 +4456,50 @@
         <v>2</v>
       </c>
       <c r="O38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P38">
+        <f>2*Tableau9[[#This Row],[Par robot :]]</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G39" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H39">
         <v>2</v>
       </c>
       <c r="O39">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P39">
+        <f>2*Tableau9[[#This Row],[Par robot :]]</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>97</v>
       </c>
       <c r="G40" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="I40">
         <v>1</v>
       </c>
       <c r="O40">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <f>2*Tableau9[[#This Row],[Par robot :]]</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>0</v>
       </c>
@@ -4233,7 +4516,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>2</v>
       </c>
@@ -4247,10 +4530,10 @@
         <v>1</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>5</v>
       </c>
@@ -4264,10 +4547,10 @@
         <v>1</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>7</v>
       </c>
@@ -4284,7 +4567,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>8</v>
       </c>
@@ -4298,10 +4581,10 @@
         <v>1</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>9</v>
       </c>
@@ -4318,7 +4601,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>10</v>
       </c>
@@ -4332,10 +4615,10 @@
         <v>1</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>11</v>
       </c>
@@ -4352,7 +4635,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>12</v>
       </c>
@@ -4366,10 +4649,10 @@
         <v>1</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>13</v>
       </c>
@@ -4383,10 +4666,10 @@
         <v>1</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>15</v>
       </c>
@@ -4403,7 +4686,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>16</v>
       </c>
@@ -4417,10 +4700,10 @@
         <v>1</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>18</v>
       </c>
@@ -4434,10 +4717,10 @@
         <v>1</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>19</v>
       </c>
@@ -4454,13 +4737,13 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>0</v>
       </c>
@@ -4477,7 +4760,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>1</v>
       </c>
@@ -4491,10 +4774,10 @@
         <v>1</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>2</v>
       </c>
@@ -4511,7 +4794,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>3</v>
       </c>
@@ -4525,10 +4808,10 @@
         <v>1</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>4</v>
       </c>
@@ -4542,10 +4825,10 @@
         <v>1</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>5</v>
       </c>
@@ -4562,7 +4845,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>6</v>
       </c>
@@ -4579,7 +4862,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>8</v>
       </c>
@@ -4596,7 +4879,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>9</v>
       </c>
@@ -4613,7 +4896,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>10</v>
       </c>
@@ -4630,7 +4913,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>11</v>
       </c>
@@ -4644,10 +4927,10 @@
         <v>1</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>12</v>
       </c>
@@ -4664,7 +4947,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>14</v>
       </c>
@@ -4681,7 +4964,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>15</v>
       </c>
@@ -4698,7 +4981,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>16</v>
       </c>
@@ -4715,7 +4998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>17</v>
       </c>
@@ -4729,10 +5012,10 @@
         <v>1</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>18</v>
       </c>
@@ -4749,7 +5032,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>19</v>
       </c>
@@ -4766,7 +5049,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>21</v>
       </c>
@@ -4783,7 +5066,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>22</v>
       </c>
@@ -4800,13 +5083,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>0</v>
       </c>
@@ -4823,7 +5106,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>2</v>
       </c>
@@ -4837,10 +5120,10 @@
         <v>1</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>3</v>
       </c>
@@ -4857,7 +5140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>4</v>
       </c>
@@ -4874,7 +5157,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>5</v>
       </c>
@@ -4891,7 +5174,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>6</v>
       </c>
@@ -4908,7 +5191,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>7</v>
       </c>
@@ -4925,7 +5208,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>8</v>
       </c>
@@ -4939,10 +5222,10 @@
         <v>2</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>9</v>
       </c>
@@ -4959,7 +5242,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>12</v>
       </c>
@@ -4973,10 +5256,10 @@
         <v>1</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>13</v>
       </c>
@@ -4993,7 +5276,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>14</v>
       </c>
@@ -5010,7 +5293,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>15</v>
       </c>
@@ -5027,7 +5310,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>16</v>
       </c>
@@ -5044,7 +5327,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>17</v>
       </c>
@@ -5061,7 +5344,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="9" t="s">
         <v>161</v>
@@ -5076,13 +5359,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>0</v>
       </c>
@@ -5099,12 +5382,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>1</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>77</v>
@@ -5116,12 +5399,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>2</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>54</v>
@@ -5130,32 +5413,32 @@
         <v>2</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>3</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D102" s="6">
         <v>1</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>4</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>57</v>
@@ -5164,10 +5447,10 @@
         <v>1</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>5</v>
       </c>
@@ -5175,21 +5458,21 @@
         <v>17</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D104" s="6">
         <v>1</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>7</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>3</v>
@@ -5201,7 +5484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>8</v>
       </c>
@@ -5209,16 +5492,16 @@
         <v>127</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D106" s="6">
         <v>1</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>9</v>
       </c>
@@ -5235,10 +5518,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5"/>
       <c r="B108" s="15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C108" s="15" t="s">
         <v>102</v>
@@ -5248,12 +5531,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
         <v>12</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>102</v>
@@ -5265,12 +5548,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="6">
         <v>2</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>54</v>
@@ -5279,11 +5562,18 @@
         <v>2</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>